<commit_message>
feat(JVM-GC): update byte code Excel file
#36
</commit_message>
<xml_diff>
--- a/28-jvm/byte-code.xlsx
+++ b/28-jvm/byte-code.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - st.sdju.edu.cn\Learning\28-jvm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5280048-90CD-467B-A277-D0C606A34C5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28318702-01CD-4E55-B824-07D1BCADA842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{50A0ADDF-1EAE-4D6F-B371-9876405451EB}"/>
   </bookViews>
@@ -619,12 +619,64 @@
         </r>
       </text>
     </comment>
+    <comment ref="J19" authorId="0" shapeId="0" xr:uid="{C8AF02F5-57C7-4798-8115-3002AF1D29EC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>小越越:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+mehtod1 code attribute end position</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E24" authorId="0" shapeId="0" xr:uid="{8E410D41-38EC-4496-A024-20D13B84A408}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>小越越:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+method2 code attribute end position</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="104">
   <si>
     <t>CA</t>
   </si>
@@ -738,6 +790,269 @@
   <si>
     <t>constant_pool</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>access_flag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>this_class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>super_class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interfaces_count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>com/deltav/Demo</t>
+  </si>
+  <si>
+    <t>java/lang/Object</t>
+  </si>
+  <si>
+    <t>field_count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>field -&gt; access_flag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>private</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>field -&gt; name_index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>field -&gt; descriptor_index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>field -&gt; attributes_count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>method count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACC_PUBLIC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name_index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;init&gt;</t>
+  </si>
+  <si>
+    <t>descriptor_index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>()V</t>
+  </si>
+  <si>
+    <t>attributes_count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attribute_name_index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>attribute_length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x38</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x52</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x08</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_stack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_local</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code_length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exception_table_length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attribute_count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LineNumberTable</t>
+  </si>
+  <si>
+    <t>line_number_table_length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>start_pc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>line_number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LocalVariableTable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>local_variable_table_lenght</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>this</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lcom/deltav/Demo;</t>
+  </si>
+  <si>
+    <t>index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Methods</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute -&gt; Code </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attribute -&gt; Code -&gt;Attribute</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attributes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SourceFile</t>
+  </si>
+  <si>
+    <t>sourcefile_index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Demo.java</t>
   </si>
 </sst>
 </file>
@@ -745,9 +1060,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="00"/>
+    <numFmt numFmtId="176" formatCode="00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -791,8 +1106,17 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="45">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -819,6 +1143,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -837,12 +1167,222 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF768A92"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEAF96"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6CECE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB27272"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0463E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDFFA7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6EA00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAC924"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBCC23C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF91953D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBFC70"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB3FD2F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF82D20C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8BAA06"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF48FD35"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6EC864"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF429051"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF47713F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF77E99D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF67C797"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF46A852"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0CDE9D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF88CAB6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2AA8A2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC3D1EF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3CC2CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7399B9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF936FE3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -850,32 +1390,112 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
@@ -884,25 +1504,307 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="26" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="30" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="31" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="32" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="41" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="42" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="43" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="44" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="4" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -911,6 +1813,20 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF936FE3"/>
+      <color rgb="FF7399B9"/>
+      <color rgb="FF3CC2CC"/>
+      <color rgb="FFC3D1EF"/>
+      <color rgb="FF2AA8A2"/>
+      <color rgb="FF88CAB6"/>
+      <color rgb="FF0CDE9D"/>
+      <color rgb="FF46A852"/>
+      <color rgb="FF67C797"/>
+      <color rgb="FF77E99D"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1223,16 +2139,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48417919-AF46-41D4-9E48-D1F8D49F06C8}">
-  <dimension ref="A1:V58"/>
+  <dimension ref="A1:Y63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="20" max="20" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.6640625" style="8"/>
+    <col min="20" max="20" width="23" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.6640625" style="41"/>
+    <col min="22" max="22" width="17.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
@@ -1248,10 +2166,10 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9">
-        <v>0</v>
-      </c>
-      <c r="F1" s="9">
+      <c r="E1" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1" s="10">
         <v>0</v>
       </c>
       <c r="G1" s="4">
@@ -1266,22 +2184,22 @@
       <c r="J1" s="6">
         <v>16</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="11">
-        <v>0</v>
-      </c>
-      <c r="M1" s="11">
+      <c r="L1" s="12">
+        <v>0</v>
+      </c>
+      <c r="M1" s="12">
         <v>4</v>
       </c>
-      <c r="N1" s="11">
-        <v>0</v>
-      </c>
-      <c r="O1" s="11">
+      <c r="N1" s="12">
+        <v>0</v>
+      </c>
+      <c r="O1" s="12">
         <v>12</v>
       </c>
-      <c r="P1" s="13">
+      <c r="P1" s="14">
         <v>9</v>
       </c>
       <c r="T1" s="3" t="s">
@@ -1289,912 +2207,969 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
-        <v>0</v>
-      </c>
-      <c r="B2" s="13">
+      <c r="A2" s="14">
+        <v>0</v>
+      </c>
+      <c r="B2" s="14">
         <v>3</v>
       </c>
-      <c r="C2" s="13">
-        <v>0</v>
-      </c>
-      <c r="D2" s="13">
+      <c r="C2" s="14">
+        <v>0</v>
+      </c>
+      <c r="D2" s="14">
         <v>13</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="12">
         <v>7</v>
       </c>
-      <c r="F2" s="11">
-        <v>0</v>
-      </c>
-      <c r="G2" s="11">
+      <c r="F2" s="12">
+        <v>0</v>
+      </c>
+      <c r="G2" s="12">
         <v>14</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="14">
         <v>7</v>
       </c>
-      <c r="I2" s="13">
-        <v>0</v>
-      </c>
-      <c r="J2" s="13">
+      <c r="I2" s="14">
+        <v>0</v>
+      </c>
+      <c r="J2" s="14">
         <v>15</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="12">
         <v>1</v>
       </c>
-      <c r="L2" s="11">
-        <v>0</v>
-      </c>
-      <c r="M2" s="11">
+      <c r="L2" s="12">
+        <v>0</v>
+      </c>
+      <c r="M2" s="12">
         <v>3</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="N2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="11">
+      <c r="O2" s="12">
         <v>75</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="P2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="10" t="s">
+      <c r="T2" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+      <c r="A3" s="14">
         <v>1</v>
       </c>
-      <c r="B3" s="13">
-        <v>0</v>
-      </c>
-      <c r="C3" s="13">
+      <c r="B3" s="14">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14">
         <v>1</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="14">
         <v>49</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="12">
         <v>1</v>
       </c>
-      <c r="F3" s="11">
-        <v>0</v>
-      </c>
-      <c r="G3" s="11">
+      <c r="F3" s="12">
+        <v>0</v>
+      </c>
+      <c r="G3" s="12">
         <v>6</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="12">
         <v>69</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="12">
         <v>69</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="12">
         <v>74</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="13">
+      <c r="N3" s="14">
         <v>1</v>
       </c>
-      <c r="O3" s="13">
-        <v>0</v>
-      </c>
-      <c r="P3" s="13">
+      <c r="O3" s="14">
+        <v>0</v>
+      </c>
+      <c r="P3" s="14">
         <v>3</v>
       </c>
       <c r="T3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="U3">
-        <v>52</v>
+      <c r="U3" s="41" t="s">
+        <v>63</v>
       </c>
       <c r="V3" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+      <c r="A4" s="14">
         <v>28</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="14">
         <v>29</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="14">
         <v>56</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="12">
         <v>1</v>
       </c>
-      <c r="E4" s="11">
-        <v>0</v>
-      </c>
-      <c r="F4" s="11">
+      <c r="E4" s="12">
+        <v>0</v>
+      </c>
+      <c r="F4" s="12">
         <v>4</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="12">
         <v>43</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="12">
         <v>64</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="12">
         <v>65</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="14">
         <v>1</v>
       </c>
-      <c r="L4" s="13">
-        <v>0</v>
-      </c>
-      <c r="M4" s="13" t="s">
+      <c r="L4" s="14">
+        <v>0</v>
+      </c>
+      <c r="M4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="13" t="s">
+      <c r="N4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="13">
+      <c r="O4" s="14">
         <v>69</v>
       </c>
-      <c r="P4" s="13" t="s">
+      <c r="P4" s="14" t="s">
         <v>5</v>
       </c>
       <c r="T4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="U4">
-        <v>22</v>
+      <c r="U4" s="41" t="s">
+        <v>64</v>
       </c>
       <c r="V4" s="8">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="14">
         <v>65</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="14">
         <v>75</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="14">
         <v>62</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="14">
         <v>65</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="14">
         <v>72</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="14">
         <v>54</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="14">
         <v>61</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="14">
         <v>62</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="14">
         <v>65</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="12">
         <v>1</v>
       </c>
-      <c r="N5" s="11">
-        <v>0</v>
-      </c>
-      <c r="O5" s="11">
+      <c r="N5" s="12">
+        <v>0</v>
+      </c>
+      <c r="O5" s="12">
         <v>12</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="P5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="T5" s="12" t="s">
+      <c r="T5" s="13" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="12">
         <v>63</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="12">
         <v>61</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="12">
         <v>56</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="12">
         <v>61</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="12">
         <v>72</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="12">
         <v>69</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="12">
         <v>61</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="12">
         <v>62</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="12">
         <v>65</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="12">
         <v>54</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="12">
         <v>61</v>
       </c>
-      <c r="O6" s="11">
+      <c r="O6" s="12">
         <v>62</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="P6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="T6" s="14" t="s">
+      <c r="T6" s="15" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
+      <c r="A7" s="12">
         <v>65</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="14">
         <v>1</v>
       </c>
-      <c r="C7" s="13">
-        <v>0</v>
-      </c>
-      <c r="D7" s="13">
+      <c r="C7" s="14">
+        <v>0</v>
+      </c>
+      <c r="D7" s="14">
         <v>4</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="14">
         <v>74</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="14">
         <v>68</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="14">
         <v>69</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="14">
         <v>73</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="12">
         <v>1</v>
       </c>
-      <c r="J7" s="11">
-        <v>0</v>
-      </c>
-      <c r="K7" s="11">
+      <c r="J7" s="12">
+        <v>0</v>
+      </c>
+      <c r="K7" s="12">
         <v>11</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="L7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="12">
         <v>63</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="N7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="11" t="s">
+      <c r="O7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="P7" s="11" t="s">
+      <c r="P7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="T7" s="15"/>
+      <c r="T7" s="18"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
+      <c r="A8" s="12">
         <v>64</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="12">
         <v>65</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="12">
         <v>74</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="12">
         <v>61</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="12">
         <v>76</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="12">
         <v>44</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="12">
         <v>65</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="11" t="s">
+      <c r="L8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="14">
         <v>1</v>
       </c>
-      <c r="N8" s="13">
-        <v>0</v>
-      </c>
-      <c r="O8" s="13">
+      <c r="N8" s="14">
+        <v>0</v>
+      </c>
+      <c r="O8" s="14">
         <v>3</v>
       </c>
-      <c r="P8" s="13">
+      <c r="P8" s="14">
         <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="14">
         <v>64</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="14">
         <v>64</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="12">
         <v>1</v>
       </c>
-      <c r="D9" s="11">
-        <v>0</v>
-      </c>
-      <c r="E9" s="11">
+      <c r="D9" s="12">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12">
         <v>3</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="12">
         <v>28</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="12">
         <v>29</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="12">
         <v>49</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="14">
         <v>1</v>
       </c>
-      <c r="J9" s="13">
-        <v>0</v>
-      </c>
-      <c r="K9" s="13" t="s">
+      <c r="J9" s="14">
+        <v>0</v>
+      </c>
+      <c r="K9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="14">
         <v>53</v>
       </c>
-      <c r="M9" s="13" t="s">
+      <c r="M9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N9" s="13">
+      <c r="N9" s="14">
         <v>75</v>
       </c>
-      <c r="O9" s="13">
+      <c r="O9" s="14">
         <v>72</v>
       </c>
-      <c r="P9" s="13">
+      <c r="P9" s="14">
         <v>63</v>
       </c>
+      <c r="T9" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="U9" s="41" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="A10" s="14">
         <v>65</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="14">
         <v>46</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="14">
         <v>69</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="14">
         <v>65</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="12">
         <v>1</v>
       </c>
-      <c r="G10" s="11">
-        <v>0</v>
-      </c>
-      <c r="H10" s="11">
+      <c r="G10" s="12">
+        <v>0</v>
+      </c>
+      <c r="H10" s="12">
         <v>9</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="12">
         <v>44</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="12">
         <v>65</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="L10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="M10" s="11" t="s">
+      <c r="M10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="11" t="s">
+      <c r="N10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="O10" s="11">
+      <c r="O10" s="12">
         <v>61</v>
       </c>
-      <c r="P10" s="11">
+      <c r="P10" s="12">
         <v>76</v>
       </c>
+      <c r="T10" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="U10" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="V10" s="8" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
+      <c r="A11" s="12">
         <v>61</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="13">
-        <v>0</v>
-      </c>
-      <c r="D11" s="13">
+      <c r="C11" s="14">
+        <v>0</v>
+      </c>
+      <c r="D11" s="14">
         <v>7</v>
       </c>
-      <c r="E11" s="13">
-        <v>0</v>
-      </c>
-      <c r="F11" s="13">
+      <c r="E11" s="14">
+        <v>0</v>
+      </c>
+      <c r="F11" s="14">
         <v>8</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0</v>
+      </c>
+      <c r="I11" s="12">
+        <v>5</v>
+      </c>
+      <c r="J11" s="12">
+        <v>0</v>
+      </c>
+      <c r="K11" s="12">
+        <v>6</v>
+      </c>
+      <c r="L11" s="14">
+        <v>1</v>
+      </c>
+      <c r="M11" s="14">
+        <v>0</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" s="14">
+        <v>63</v>
+      </c>
+      <c r="P11" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="T11" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="U11" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="V11" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="14">
+        <v>64</v>
+      </c>
+      <c r="D12" s="14">
+        <v>65</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="14">
+        <v>74</v>
+      </c>
+      <c r="G12" s="14">
+        <v>61</v>
+      </c>
+      <c r="H12" s="14">
+        <v>76</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="14">
+        <v>44</v>
+      </c>
+      <c r="K12" s="14">
+        <v>65</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" s="12">
+        <v>1</v>
+      </c>
+      <c r="O12" s="12">
+        <v>0</v>
+      </c>
+      <c r="P12" s="12">
+        <v>10</v>
+      </c>
+      <c r="T12" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="12">
+        <v>61</v>
+      </c>
+      <c r="C13" s="12">
+        <v>76</v>
+      </c>
+      <c r="D13" s="12">
+        <v>61</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="12">
+        <v>61</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="12">
+        <v>67</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="12">
+        <v>62</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N13" s="12">
+        <v>65</v>
+      </c>
+      <c r="O13" s="12">
+        <v>63</v>
+      </c>
+      <c r="P13" s="12">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="16">
+        <v>0</v>
+      </c>
+      <c r="B14" s="16">
+        <v>21</v>
+      </c>
+      <c r="C14" s="19">
+        <v>0</v>
+      </c>
+      <c r="D14" s="19">
+        <v>3</v>
+      </c>
+      <c r="E14" s="21">
+        <v>0</v>
+      </c>
+      <c r="F14" s="21">
+        <v>4</v>
+      </c>
+      <c r="G14" s="23">
+        <v>0</v>
+      </c>
+      <c r="H14" s="23">
+        <v>0</v>
+      </c>
+      <c r="I14" s="25">
+        <v>0</v>
+      </c>
+      <c r="J14" s="25">
+        <v>1</v>
+      </c>
+      <c r="K14" s="9">
+        <v>0</v>
+      </c>
+      <c r="L14" s="9">
+        <v>2</v>
+      </c>
+      <c r="M14" s="27">
+        <v>0</v>
+      </c>
+      <c r="N14" s="27">
+        <v>5</v>
+      </c>
+      <c r="O14" s="30">
+        <v>0</v>
+      </c>
+      <c r="P14" s="30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="32">
+        <v>0</v>
+      </c>
+      <c r="B15" s="32">
+        <v>0</v>
+      </c>
+      <c r="C15" s="34">
+        <v>0</v>
+      </c>
+      <c r="D15" s="34">
+        <v>2</v>
+      </c>
+      <c r="E15" s="35">
+        <v>0</v>
+      </c>
+      <c r="F15" s="35">
+        <v>1</v>
+      </c>
+      <c r="G15" s="36">
+        <v>0</v>
+      </c>
+      <c r="H15" s="36">
+        <v>7</v>
+      </c>
+      <c r="I15" s="37">
+        <v>0</v>
+      </c>
+      <c r="J15" s="37">
+        <v>8</v>
+      </c>
+      <c r="K15" s="38">
+        <v>0</v>
+      </c>
+      <c r="L15" s="38">
+        <v>1</v>
+      </c>
+      <c r="M15" s="39">
+        <v>0</v>
+      </c>
+      <c r="N15" s="39">
+        <v>9</v>
+      </c>
+      <c r="O15" s="40">
+        <v>0</v>
+      </c>
+      <c r="P15" s="40">
+        <v>0</v>
+      </c>
+      <c r="T15" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="40">
+        <v>0</v>
+      </c>
+      <c r="B16" s="40">
+        <v>38</v>
+      </c>
+      <c r="C16" s="42">
+        <v>0</v>
+      </c>
+      <c r="D16" s="42">
+        <v>2</v>
+      </c>
+      <c r="E16" s="43">
+        <v>0</v>
+      </c>
+      <c r="F16" s="43">
+        <v>1</v>
+      </c>
+      <c r="G16" s="44">
+        <v>0</v>
+      </c>
+      <c r="H16" s="44">
+        <v>0</v>
+      </c>
+      <c r="I16" s="44">
+        <v>0</v>
+      </c>
+      <c r="J16" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" s="45">
+        <v>0</v>
+      </c>
+      <c r="N16" s="45">
+        <v>1</v>
+      </c>
+      <c r="O16" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="P16" s="45">
+        <v>4</v>
+      </c>
+      <c r="T16" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="U16" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="V16" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A17" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="45">
+        <v>0</v>
+      </c>
+      <c r="C17" s="45">
+        <v>2</v>
+      </c>
+      <c r="D17" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="46">
+        <v>0</v>
+      </c>
+      <c r="F17" s="46">
+        <v>0</v>
+      </c>
+      <c r="G17" s="47">
+        <v>0</v>
+      </c>
+      <c r="H17" s="47">
+        <v>2</v>
+      </c>
+      <c r="I17" s="48">
+        <v>0</v>
+      </c>
+      <c r="J17" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" s="49">
+        <v>0</v>
+      </c>
+      <c r="L17" s="49">
+        <v>0</v>
+      </c>
+      <c r="M17" s="49">
+        <v>0</v>
+      </c>
+      <c r="N17" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="O17" s="50">
+        <v>0</v>
+      </c>
+      <c r="P17" s="50">
+        <v>2</v>
+      </c>
+      <c r="T17" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="U17" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="V17" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A18" s="51">
+        <v>0</v>
+      </c>
+      <c r="B18" s="51">
+        <v>0</v>
+      </c>
+      <c r="C18" s="52">
+        <v>0</v>
+      </c>
+      <c r="D18" s="52">
+        <v>9</v>
+      </c>
+      <c r="E18" s="51">
+        <v>0</v>
+      </c>
+      <c r="F18" s="51">
+        <v>4</v>
+      </c>
+      <c r="G18" s="52">
+        <v>0</v>
+      </c>
+      <c r="H18" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" s="48">
+        <v>0</v>
+      </c>
+      <c r="J18" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="K18" s="49">
+        <v>0</v>
+      </c>
+      <c r="L18" s="49">
+        <v>0</v>
+      </c>
+      <c r="M18" s="49">
+        <v>0</v>
+      </c>
+      <c r="N18" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="11">
-        <v>0</v>
-      </c>
-      <c r="I11" s="11">
-        <v>5</v>
-      </c>
-      <c r="J11" s="11">
-        <v>0</v>
-      </c>
-      <c r="K11" s="11">
-        <v>6</v>
-      </c>
-      <c r="L11" s="13">
+      <c r="O18" s="53">
+        <v>0</v>
+      </c>
+      <c r="P18" s="53">
         <v>1</v>
       </c>
-      <c r="M11" s="13">
-        <v>0</v>
-      </c>
-      <c r="N11" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="O11" s="13">
-        <v>63</v>
-      </c>
-      <c r="P11" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="13">
-        <v>64</v>
-      </c>
-      <c r="D12" s="13">
-        <v>65</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="13">
-        <v>74</v>
-      </c>
-      <c r="G12" s="13">
-        <v>61</v>
-      </c>
-      <c r="H12" s="13">
-        <v>76</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="13">
-        <v>44</v>
-      </c>
-      <c r="K12" s="13">
-        <v>65</v>
-      </c>
-      <c r="L12" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="M12" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="N12" s="11">
-        <v>1</v>
-      </c>
-      <c r="O12" s="11">
-        <v>0</v>
-      </c>
-      <c r="P12" s="11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="11">
-        <v>61</v>
-      </c>
-      <c r="C13" s="11">
-        <v>76</v>
-      </c>
-      <c r="D13" s="11">
-        <v>61</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="11">
-        <v>61</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I13" s="11">
-        <v>67</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="L13" s="11">
-        <v>62</v>
-      </c>
-      <c r="M13" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="N13" s="11">
-        <v>65</v>
-      </c>
-      <c r="O13" s="11">
-        <v>63</v>
-      </c>
-      <c r="P13" s="11">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>0</v>
-      </c>
-      <c r="B14" s="1">
-        <v>21</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1">
-        <v>3</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1">
+      <c r="T18" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="U18" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="V18" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A19" s="54">
+        <v>0</v>
+      </c>
+      <c r="B19" s="54">
+        <v>0</v>
+      </c>
+      <c r="C19" s="55">
+        <v>0</v>
+      </c>
+      <c r="D19" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0</v>
-      </c>
-      <c r="J14" s="1">
-        <v>1</v>
-      </c>
-      <c r="K14" s="1">
-        <v>0</v>
-      </c>
-      <c r="L14" s="1">
-        <v>2</v>
-      </c>
-      <c r="M14" s="1">
-        <v>0</v>
-      </c>
-      <c r="N14" s="1">
-        <v>5</v>
-      </c>
-      <c r="O14" s="1">
-        <v>0</v>
-      </c>
-      <c r="P14" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>0</v>
-      </c>
-      <c r="B15" s="1">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1">
-        <v>2</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
-        <v>7</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1">
-        <v>8</v>
-      </c>
-      <c r="K15" s="1">
-        <v>0</v>
-      </c>
-      <c r="L15" s="1">
-        <v>1</v>
-      </c>
-      <c r="M15" s="1">
-        <v>0</v>
-      </c>
-      <c r="N15" s="1">
-        <v>9</v>
-      </c>
-      <c r="O15" s="1">
-        <v>0</v>
-      </c>
-      <c r="P15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>0</v>
-      </c>
-      <c r="B16" s="1">
-        <v>38</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1">
-        <v>2</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M16" s="1">
-        <v>0</v>
-      </c>
-      <c r="N16" s="1">
-        <v>1</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P16" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1">
-        <v>2</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1">
-        <v>2</v>
-      </c>
-      <c r="I17" s="1">
-        <v>0</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K17" s="1">
-        <v>0</v>
-      </c>
-      <c r="L17" s="1">
-        <v>0</v>
-      </c>
-      <c r="M17" s="1">
-        <v>0</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O17" s="1">
-        <v>0</v>
-      </c>
-      <c r="P17" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1">
-        <v>9</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-      <c r="F18" s="1">
-        <v>4</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I18" s="1">
-        <v>0</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" s="1">
-        <v>0</v>
-      </c>
-      <c r="L18" s="1">
-        <v>0</v>
-      </c>
-      <c r="M18" s="1">
-        <v>0</v>
-      </c>
-      <c r="N18" s="1" t="s">
+      <c r="E19" s="56">
+        <v>0</v>
+      </c>
+      <c r="F19" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="O18" s="1">
-        <v>0</v>
-      </c>
-      <c r="P18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>0</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="1">
-        <v>0</v>
-      </c>
-      <c r="H19" s="1" t="s">
+      <c r="G19" s="57">
+        <v>0</v>
+      </c>
+      <c r="H19" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="1">
-        <v>0</v>
-      </c>
-      <c r="J19" s="1">
+      <c r="I19" s="58">
+        <v>0</v>
+      </c>
+      <c r="J19" s="58">
         <v>0</v>
       </c>
       <c r="K19" s="1">
@@ -2215,8 +3190,14 @@
       <c r="P19" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T19" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="U19" s="41" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -2266,7 +3247,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -2315,8 +3296,16 @@
       <c r="P21" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T21" s="62" t="s">
+        <v>95</v>
+      </c>
+      <c r="U21" s="63"/>
+      <c r="V21" s="64"/>
+      <c r="W21" s="65"/>
+      <c r="X21" s="65"/>
+      <c r="Y21" s="66"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>0</v>
       </c>
@@ -2365,8 +3354,18 @@
       <c r="P22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T22" s="90" t="s">
+        <v>51</v>
+      </c>
+      <c r="U22" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="V22" s="60"/>
+      <c r="W22" s="61"/>
+      <c r="X22" s="61"/>
+      <c r="Y22" s="68"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
@@ -2415,8 +3414,20 @@
       <c r="P23" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T23" s="91" t="s">
+        <v>37</v>
+      </c>
+      <c r="U23" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="V23" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="W23" s="61"/>
+      <c r="X23" s="61"/>
+      <c r="Y23" s="68"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
@@ -2432,39 +3443,51 @@
       <c r="E24" s="1">
         <v>0</v>
       </c>
-      <c r="F24" s="1">
-        <v>0</v>
-      </c>
-      <c r="G24" s="1">
+      <c r="F24" s="98">
+        <v>0</v>
+      </c>
+      <c r="G24" s="98">
         <v>1</v>
       </c>
-      <c r="H24" s="1">
-        <v>0</v>
-      </c>
-      <c r="I24" s="1">
+      <c r="H24" s="99">
+        <v>0</v>
+      </c>
+      <c r="I24" s="99">
         <v>10</v>
       </c>
-      <c r="J24" s="1">
-        <v>0</v>
-      </c>
-      <c r="K24" s="1">
-        <v>0</v>
-      </c>
-      <c r="L24" s="1">
-        <v>0</v>
-      </c>
-      <c r="M24" s="1">
+      <c r="J24" s="100">
+        <v>0</v>
+      </c>
+      <c r="K24" s="100">
+        <v>0</v>
+      </c>
+      <c r="L24" s="100">
+        <v>0</v>
+      </c>
+      <c r="M24" s="100">
         <v>2</v>
       </c>
-      <c r="N24" s="1">
-        <v>0</v>
-      </c>
-      <c r="O24" s="1">
+      <c r="N24" s="101">
+        <v>0</v>
+      </c>
+      <c r="O24" s="101">
         <v>11</v>
       </c>
       <c r="P24" s="1"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T24" s="92" t="s">
+        <v>53</v>
+      </c>
+      <c r="U24" s="59" t="s">
+        <v>73</v>
+      </c>
+      <c r="V24" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="W24" s="61"/>
+      <c r="X24" s="61"/>
+      <c r="Y24" s="68"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2481,8 +3504,20 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T25" s="93" t="s">
+        <v>55</v>
+      </c>
+      <c r="U25" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="V25" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="W25" s="61"/>
+      <c r="X25" s="61"/>
+      <c r="Y25" s="68"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2499,8 +3534,18 @@
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T26" s="94" t="s">
+        <v>57</v>
+      </c>
+      <c r="U26" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="V26" s="60"/>
+      <c r="W26" s="61"/>
+      <c r="X26" s="61"/>
+      <c r="Y26" s="68"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2517,8 +3562,14 @@
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T27" s="95"/>
+      <c r="U27" s="59"/>
+      <c r="V27" s="60"/>
+      <c r="W27" s="61"/>
+      <c r="X27" s="61"/>
+      <c r="Y27" s="68"/>
+    </row>
+    <row r="28" spans="1:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2535,8 +3586,14 @@
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T28" s="95"/>
+      <c r="U28" s="59"/>
+      <c r="V28" s="60"/>
+      <c r="W28" s="61"/>
+      <c r="X28" s="61"/>
+      <c r="Y28" s="68"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2553,8 +3610,16 @@
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T29" s="62" t="s">
+        <v>96</v>
+      </c>
+      <c r="U29" s="63"/>
+      <c r="V29" s="64"/>
+      <c r="W29" s="65"/>
+      <c r="X29" s="66"/>
+      <c r="Y29" s="68"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2571,8 +3636,20 @@
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T30" s="67" t="s">
+        <v>58</v>
+      </c>
+      <c r="U30" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="V30" s="60" t="s">
+        <v>59</v>
+      </c>
+      <c r="W30" s="61"/>
+      <c r="X30" s="68"/>
+      <c r="Y30" s="68"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2589,8 +3666,20 @@
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T31" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="U31" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="V31" s="60">
+        <v>56</v>
+      </c>
+      <c r="W31" s="61"/>
+      <c r="X31" s="68"/>
+      <c r="Y31" s="68"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2607,8 +3696,20 @@
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T32" s="70" t="s">
+        <v>75</v>
+      </c>
+      <c r="U32" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="V32" s="60">
+        <v>2</v>
+      </c>
+      <c r="W32" s="61"/>
+      <c r="X32" s="68"/>
+      <c r="Y32" s="68"/>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2625,8 +3726,20 @@
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T33" s="71" t="s">
+        <v>76</v>
+      </c>
+      <c r="U33" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="V33" s="60">
+        <v>1</v>
+      </c>
+      <c r="W33" s="61"/>
+      <c r="X33" s="68"/>
+      <c r="Y33" s="68"/>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2643,8 +3756,20 @@
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T34" s="72" t="s">
+        <v>77</v>
+      </c>
+      <c r="U34" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="V34" s="60">
+        <v>10</v>
+      </c>
+      <c r="W34" s="61"/>
+      <c r="X34" s="68"/>
+      <c r="Y34" s="68"/>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2661,8 +3786,16 @@
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T35" s="73" t="s">
+        <v>79</v>
+      </c>
+      <c r="U35" s="59"/>
+      <c r="V35" s="60"/>
+      <c r="W35" s="61"/>
+      <c r="X35" s="68"/>
+      <c r="Y35" s="68"/>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2679,8 +3812,20 @@
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T36" s="74" t="s">
+        <v>80</v>
+      </c>
+      <c r="U36" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="V36" s="60">
+        <v>0</v>
+      </c>
+      <c r="W36" s="61"/>
+      <c r="X36" s="68"/>
+      <c r="Y36" s="68"/>
+    </row>
+    <row r="37" spans="1:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2697,8 +3842,20 @@
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T37" s="75" t="s">
+        <v>81</v>
+      </c>
+      <c r="U37" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="V37" s="60">
+        <v>2</v>
+      </c>
+      <c r="W37" s="61"/>
+      <c r="X37" s="68"/>
+      <c r="Y37" s="68"/>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2715,8 +3872,16 @@
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T38" s="62" t="s">
+        <v>97</v>
+      </c>
+      <c r="U38" s="63"/>
+      <c r="V38" s="64"/>
+      <c r="W38" s="66"/>
+      <c r="X38" s="68"/>
+      <c r="Y38" s="68"/>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2733,8 +3898,22 @@
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T39" s="76" t="s">
+        <v>58</v>
+      </c>
+      <c r="U39" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="V39" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="W39" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="X39" s="68"/>
+      <c r="Y39" s="68"/>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2751,8 +3930,22 @@
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T40" s="77" t="s">
+        <v>60</v>
+      </c>
+      <c r="U40" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="V40" s="60">
+        <v>10</v>
+      </c>
+      <c r="W40" s="68">
+        <v>13</v>
+      </c>
+      <c r="X40" s="68"/>
+      <c r="Y40" s="68"/>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2769,8 +3962,20 @@
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T41" s="78" t="s">
+        <v>83</v>
+      </c>
+      <c r="U41" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="V41" s="60">
+        <v>2</v>
+      </c>
+      <c r="W41" s="68"/>
+      <c r="X41" s="68"/>
+      <c r="Y41" s="68"/>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2787,8 +3992,16 @@
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T42" s="79" t="s">
+        <v>84</v>
+      </c>
+      <c r="U42" s="59"/>
+      <c r="V42" s="60"/>
+      <c r="W42" s="68"/>
+      <c r="X42" s="68"/>
+      <c r="Y42" s="68"/>
+    </row>
+    <row r="43" spans="1:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2805,8 +4018,16 @@
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T43" s="97" t="s">
+        <v>85</v>
+      </c>
+      <c r="U43" s="87"/>
+      <c r="V43" s="88"/>
+      <c r="W43" s="89"/>
+      <c r="X43" s="68"/>
+      <c r="Y43" s="68"/>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2823,8 +4044,16 @@
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T44" s="62" t="s">
+        <v>97</v>
+      </c>
+      <c r="U44" s="63"/>
+      <c r="V44" s="64"/>
+      <c r="W44" s="66"/>
+      <c r="X44" s="68"/>
+      <c r="Y44" s="68"/>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2841,8 +4070,20 @@
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T45" s="80" t="s">
+        <v>88</v>
+      </c>
+      <c r="U45" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="V45" s="60">
+        <v>1</v>
+      </c>
+      <c r="W45" s="68"/>
+      <c r="X45" s="68"/>
+      <c r="Y45" s="68"/>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2859,8 +4100,20 @@
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T46" s="81" t="s">
+        <v>84</v>
+      </c>
+      <c r="U46" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="V46" s="60">
+        <v>0</v>
+      </c>
+      <c r="W46" s="68"/>
+      <c r="X46" s="68"/>
+      <c r="Y46" s="68"/>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2877,8 +4130,20 @@
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T47" s="82" t="s">
+        <v>89</v>
+      </c>
+      <c r="U47" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="V47" s="60">
+        <v>10</v>
+      </c>
+      <c r="W47" s="68"/>
+      <c r="X47" s="68"/>
+      <c r="Y47" s="68"/>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2895,8 +4160,20 @@
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T48" s="83" t="s">
+        <v>53</v>
+      </c>
+      <c r="U48" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="V48" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="W48" s="68"/>
+      <c r="X48" s="68"/>
+      <c r="Y48" s="68"/>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2913,8 +4190,20 @@
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T49" s="84" t="s">
+        <v>55</v>
+      </c>
+      <c r="U49" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="V49" s="60" t="s">
+        <v>93</v>
+      </c>
+      <c r="W49" s="68"/>
+      <c r="X49" s="68"/>
+      <c r="Y49" s="68"/>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2931,8 +4220,20 @@
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T50" s="85" t="s">
+        <v>94</v>
+      </c>
+      <c r="U50" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="V50" s="60">
+        <v>0</v>
+      </c>
+      <c r="W50" s="68"/>
+      <c r="X50" s="68"/>
+      <c r="Y50" s="68"/>
+    </row>
+    <row r="51" spans="1:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2949,8 +4250,14 @@
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T51" s="86"/>
+      <c r="U51" s="87"/>
+      <c r="V51" s="88"/>
+      <c r="W51" s="89"/>
+      <c r="X51" s="68"/>
+      <c r="Y51" s="68"/>
+    </row>
+    <row r="52" spans="1:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2967,8 +4274,14 @@
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T52" s="86"/>
+      <c r="U52" s="87"/>
+      <c r="V52" s="88"/>
+      <c r="W52" s="96"/>
+      <c r="X52" s="89"/>
+      <c r="Y52" s="68"/>
+    </row>
+    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2985,8 +4298,14 @@
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T53" s="95"/>
+      <c r="U53" s="59"/>
+      <c r="V53" s="60"/>
+      <c r="W53" s="61"/>
+      <c r="X53" s="61"/>
+      <c r="Y53" s="68"/>
+    </row>
+    <row r="54" spans="1:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -3003,8 +4322,14 @@
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T54" s="86"/>
+      <c r="U54" s="87"/>
+      <c r="V54" s="88"/>
+      <c r="W54" s="96"/>
+      <c r="X54" s="96"/>
+      <c r="Y54" s="89"/>
+    </row>
+    <row r="55" spans="1:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -3022,7 +4347,7 @@
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -3039,8 +4364,12 @@
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T56" s="108"/>
+      <c r="U56" s="63"/>
+      <c r="V56" s="64"/>
+      <c r="W56" s="66"/>
+    </row>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -3057,8 +4386,18 @@
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T57" s="109" t="s">
+        <v>81</v>
+      </c>
+      <c r="U57" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="V57" s="60">
+        <v>1</v>
+      </c>
+      <c r="W57" s="68"/>
+    </row>
+    <row r="58" spans="1:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -3075,6 +4414,60 @@
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
+      <c r="T58" s="95"/>
+      <c r="U58" s="59"/>
+      <c r="V58" s="60"/>
+      <c r="W58" s="68"/>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="T59" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="U59" s="63"/>
+      <c r="V59" s="102"/>
+      <c r="W59" s="68"/>
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="T60" s="103" t="s">
+        <v>58</v>
+      </c>
+      <c r="U60" s="59" t="s">
+        <v>99</v>
+      </c>
+      <c r="V60" s="104" t="s">
+        <v>100</v>
+      </c>
+      <c r="W60" s="68"/>
+    </row>
+    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="T61" s="105" t="s">
+        <v>60</v>
+      </c>
+      <c r="U61" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="V61" s="104">
+        <v>2</v>
+      </c>
+      <c r="W61" s="68"/>
+    </row>
+    <row r="62" spans="1:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T62" s="106" t="s">
+        <v>101</v>
+      </c>
+      <c r="U62" s="87" t="s">
+        <v>102</v>
+      </c>
+      <c r="V62" s="107" t="s">
+        <v>103</v>
+      </c>
+      <c r="W62" s="68"/>
+    </row>
+    <row r="63" spans="1:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T63" s="86"/>
+      <c r="U63" s="87"/>
+      <c r="V63" s="88"/>
+      <c r="W63" s="89"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>